<commit_message>
Pushed commit with wrong message, file contains split chr pos and no from original data file
</commit_message>
<xml_diff>
--- a/Data/DRIP_seq_data_IIHG-tidied-2.28.2023-Sherrin.xlsx
+++ b/Data/DRIP_seq_data_IIHG-tidied-2.28.2023-Sherrin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarahicks/Documents/ISC/Final_project/biol-4386-course-project-tarahicks/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4EC77A-7AE4-DC47-8BDE-841358D06C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6822BF-5918-1347-821B-8772F6788CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="299">
   <si>
     <t>X</t>
   </si>
@@ -932,9 +932,6 @@
   </si>
   <si>
     <t>Total_read_number</t>
-  </si>
-  <si>
-    <t>0.09/100=</t>
   </si>
 </sst>
 </file>
@@ -1353,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3128,9 +3125,7 @@
         <f t="shared" si="1"/>
         <v>9.0872589628582315E-2</v>
       </c>
-      <c r="E110" s="6" t="s">
-        <v>299</v>
-      </c>
+      <c r="E110" s="6"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">

</xml_diff>